<commit_message>
Atualizacao da checklist e historia de casos de uso
</commit_message>
<xml_diff>
--- a/SGB/6.Gerenciamento de Projeto/Template - Checklist Verificacao de Projeto.xltx.xlsx
+++ b/SGB/6.Gerenciamento de Projeto/Template - Checklist Verificacao de Projeto.xltx.xlsx
@@ -312,7 +312,7 @@
     <t>Existe template para documento não previsto no SpinOff?</t>
   </si>
   <si>
-    <t>Sim</t>
+    <t>NA</t>
   </si>
   <si>
     <t>Desenvolvimento - Requisitos</t>
@@ -321,13 +321,13 @@
     <t>O artefato foi criado com o template atual e armazenado na pasta correta da estrutura do projeto?</t>
   </si>
   <si>
+    <t>Sim</t>
+  </si>
+  <si>
     <t>O objetivo, os problemas  e as necessidades do cliente estão claras?</t>
   </si>
   <si>
     <t>As necessidades foram descritas como histórias de usuário?</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>Fornece uma visão geral do sistema de forma clara e objetiva?</t>
@@ -340,9 +340,6 @@
   </si>
   <si>
     <t>Os casos de uso e atores possuem descrições claras e objetivas de forma a não necessitar que alguém explique-o verbalmente?</t>
-  </si>
-  <si>
-    <t>Parcialmente</t>
   </si>
   <si>
     <t>Caso tenha sido criado o protótipo, ele foi armazenado na pasta correta da estrutura do projeto?</t>
@@ -400,6 +397,9 @@
   </si>
   <si>
     <t>Os históricos de atualizações dos artefatos, na ferramenta,  possuem descrição do que foi alterado?</t>
+  </si>
+  <si>
+    <t>Parcialmente</t>
   </si>
   <si>
     <t>O visão foi atualizado devido a mudança de escopo?</t>
@@ -961,12 +961,12 @@
     <xf borderId="3" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="1" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="16" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="17" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="1" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="18" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="1" vertical="center" wrapText="0"/>
@@ -1039,11 +1039,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="2106948536"/>
-        <c:axId val="1326041783"/>
+        <c:axId val="1893046454"/>
+        <c:axId val="1816088359"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2106948536"/>
+        <c:axId val="1893046454"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1095,10 +1095,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1326041783"/>
+        <c:crossAx val="1816088359"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1326041783"/>
+        <c:axId val="1816088359"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1162,7 +1162,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2106948536"/>
+        <c:crossAx val="1893046454"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -1317,11 +1317,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="299274001"/>
-        <c:axId val="22069842"/>
+        <c:axId val="2032508185"/>
+        <c:axId val="1103735302"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="299274001"/>
+        <c:axId val="2032508185"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1373,10 +1373,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22069842"/>
+        <c:crossAx val="1103735302"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22069842"/>
+        <c:axId val="1103735302"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1440,7 +1440,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299274001"/>
+        <c:crossAx val="2032508185"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1613,11 +1613,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="301676498"/>
-        <c:axId val="707161736"/>
+        <c:axId val="115056810"/>
+        <c:axId val="1740624041"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="301676498"/>
+        <c:axId val="115056810"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1669,10 +1669,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="707161736"/>
+        <c:crossAx val="1740624041"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="707161736"/>
+        <c:axId val="1740624041"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1736,7 +1736,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="301676498"/>
+        <c:crossAx val="115056810"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1877,11 +1877,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1446145286"/>
-        <c:axId val="1203970428"/>
+        <c:axId val="1602681977"/>
+        <c:axId val="1000957750"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1446145286"/>
+        <c:axId val="1602681977"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1933,10 +1933,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1203970428"/>
+        <c:crossAx val="1000957750"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1203970428"/>
+        <c:axId val="1000957750"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1948,7 +1948,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1446145286"/>
+        <c:crossAx val="1602681977"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2089,11 +2089,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1234400800"/>
-        <c:axId val="1238937839"/>
+        <c:axId val="347069040"/>
+        <c:axId val="983789420"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1234400800"/>
+        <c:axId val="347069040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2145,10 +2145,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1238937839"/>
+        <c:crossAx val="983789420"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1238937839"/>
+        <c:axId val="983789420"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2160,7 +2160,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1234400800"/>
+        <c:crossAx val="347069040"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2566,7 +2566,7 @@
       </c>
       <c r="B3" s="5">
         <f>'Ver-Iniciação1'!$F$2</f>
-        <v>0.9090909091</v>
+        <v>0.9565217391</v>
       </c>
     </row>
     <row r="4">
@@ -5647,7 +5647,7 @@
       </c>
       <c r="B2" s="8">
         <f>('Ver-Iniciação1'!$G$5/SUM('Ver-Iniciação1'!$G$5:'Ver-Iniciação1'!$J$5))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="8">
         <f>('Ver-Iniciação1'!$H$5/SUM('Ver-Iniciação1'!$G$5:'Ver-Iniciação1'!$J$5))</f>
@@ -5659,7 +5659,7 @@
       </c>
       <c r="E2" s="8">
         <f>('Ver-Iniciação1'!$J$5/SUM('Ver-Iniciação1'!$G$5:'Ver-Iniciação1'!$J$5))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N2" s="7" t="s">
         <v>13</v>
@@ -5687,7 +5687,7 @@
       </c>
       <c r="B3" s="8">
         <f>('Ver-Iniciação1'!$G$7/SUM('Ver-Iniciação1'!$G$7:'Ver-Iniciação1'!$J$7))</f>
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="C3" s="8">
         <f>('Ver-Iniciação1'!$H$7/SUM('Ver-Iniciação1'!$G$7:'Ver-Iniciação1'!$J$7))</f>
@@ -5699,7 +5699,7 @@
       </c>
       <c r="E3" s="8">
         <f>('Ver-Iniciação1'!$J$7/SUM('Ver-Iniciação1'!$G$7:'Ver-Iniciação1'!$J$7))</f>
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="N3" s="7" t="s">
         <v>14</v>
@@ -5727,11 +5727,11 @@
       </c>
       <c r="B4" s="8">
         <f>('Ver-Iniciação1'!$G$13/SUM('Ver-Iniciação1'!$G$13:'Ver-Iniciação1'!$J$13))</f>
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="C4" s="8">
         <f>('Ver-Iniciação1'!$H$13/SUM('Ver-Iniciação1'!$G$13:'Ver-Iniciação1'!$J$13))</f>
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="D4" s="8">
         <f>('Ver-Iniciação1'!$I$13/SUM('Ver-Iniciação1'!$G$13:'Ver-Iniciação1'!$J$13))</f>
@@ -5967,11 +5967,11 @@
       </c>
       <c r="B10" s="8">
         <f>('Ver-Iniciação1'!$G$28/SUM('Ver-Iniciação1'!$G$28:'Ver-Iniciação1'!$J$28))</f>
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="C10" s="8">
         <f>('Ver-Iniciação1'!$H$28/SUM('Ver-Iniciação1'!$G$28:'Ver-Iniciação1'!$J$28))</f>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="D10" s="8">
         <f>('Ver-Iniciação1'!$I$28/SUM('Ver-Iniciação1'!$G$28:'Ver-Iniciação1'!$J$28))</f>
@@ -6011,7 +6011,7 @@
       </c>
       <c r="C11" s="8">
         <f>('Ver-Iniciação1'!$H$37/SUM('Ver-Iniciação1'!$G$37:'Ver-Iniciação1'!$J$37))</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="D11" s="8">
         <f>('Ver-Iniciação1'!$I$37/SUM('Ver-Iniciação1'!$G$37:'Ver-Iniciação1'!$J$37))</f>
@@ -6019,7 +6019,7 @@
       </c>
       <c r="E11" s="8">
         <f>('Ver-Iniciação1'!$J$37/SUM('Ver-Iniciação1'!$G$37:'Ver-Iniciação1'!$J$37))</f>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="N11" s="7" t="s">
         <v>24</v>
@@ -7637,7 +7637,7 @@
       <c r="E2" s="15"/>
       <c r="F2" s="16">
         <f>COUNTIF(D5:D41,"Sim")/(COUNTA(D5:D41)-COUNTIF(D5:D41,"NA"))</f>
-        <v>0.9090909091</v>
+        <v>0.9565217391</v>
       </c>
     </row>
     <row r="3" ht="18.75" customHeight="1">
@@ -7687,7 +7687,7 @@
       <c r="F5" s="27"/>
       <c r="G5" s="7">
         <f>COUNTIF(D6,"Sim")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="7">
         <f>COUNTIF(D6,"Parcialmente")</f>
@@ -7699,7 +7699,7 @@
       </c>
       <c r="J5" s="7">
         <f>COUNTIF(D6,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" ht="18.75" customHeight="1">
@@ -7729,7 +7729,7 @@
       <c r="F7" s="27"/>
       <c r="G7" s="7">
         <f>COUNTIF(D8:D12,"Sim")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H7" s="7">
         <f>COUNTIF(D8:D12,"Parcialmente")</f>
@@ -7741,7 +7741,7 @@
       </c>
       <c r="J7" s="7">
         <f>COUNTIF(D8:D12,"NA")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" ht="15.0" customHeight="1">
@@ -7753,7 +7753,7 @@
         <v>45</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E8" s="30"/>
       <c r="F8" s="30"/>
@@ -7764,10 +7764,10 @@
         <v>3.0</v>
       </c>
       <c r="C9" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="31" t="s">
         <v>46</v>
-      </c>
-      <c r="D9" s="31" t="s">
-        <v>43</v>
       </c>
       <c r="E9" s="30"/>
       <c r="F9" s="30"/>
@@ -7778,10 +7778,10 @@
         <v>4.0</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E10" s="30"/>
       <c r="F10" s="30"/>
@@ -7795,7 +7795,7 @@
         <v>49</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E11" s="30"/>
       <c r="F11" s="30"/>
@@ -7829,7 +7829,7 @@
         <v>50</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E12" s="30"/>
       <c r="F12" s="30"/>
@@ -7845,11 +7845,11 @@
       <c r="F13" s="27"/>
       <c r="G13" s="7">
         <f>COUNTIF(D14:D18,"Sim")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H13" s="7">
         <f>COUNTIF(D14:D18,"Parcialmente")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" s="7">
         <f>COUNTIF(D14:D18,"Não")</f>
@@ -7869,7 +7869,7 @@
         <v>45</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E14" s="30"/>
       <c r="F14" s="30"/>
@@ -7883,7 +7883,7 @@
         <v>51</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E15" s="30"/>
       <c r="F15" s="30"/>
@@ -7917,7 +7917,7 @@
         <v>52</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E16" s="30"/>
       <c r="F16" s="30"/>
@@ -7948,10 +7948,10 @@
         <v>10.0</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
@@ -7982,10 +7982,10 @@
         <v>11.0</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
@@ -8014,7 +8014,7 @@
       <c r="A19" s="32"/>
       <c r="B19" s="25"/>
       <c r="C19" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D19" s="27"/>
       <c r="E19" s="27"/>
@@ -8042,10 +8042,10 @@
         <v>12.0</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E20" s="30"/>
       <c r="F20" s="30"/>
@@ -8056,10 +8056,10 @@
         <v>13.0</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E21" s="30"/>
       <c r="F21" s="30"/>
@@ -8099,10 +8099,10 @@
         <v>45</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
+        <v>43</v>
+      </c>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
     </row>
     <row r="24" ht="18.75" customHeight="1">
       <c r="A24" s="32"/>
@@ -8110,12 +8110,12 @@
         <v>15.0</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="30"/>
+        <v>43</v>
+      </c>
+      <c r="E24" s="37"/>
       <c r="F24" s="30"/>
     </row>
     <row r="25" ht="18.75" customHeight="1">
@@ -8153,27 +8153,27 @@
         <v>45</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E26" s="30"/>
       <c r="F26" s="30"/>
     </row>
     <row r="27" ht="18.75" customHeight="1">
-      <c r="A27" s="37"/>
+      <c r="A27" s="38"/>
       <c r="B27" s="29">
         <v>17.0</v>
       </c>
       <c r="C27" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E27" s="30"/>
       <c r="F27" s="30"/>
     </row>
     <row r="28" ht="18.75" customHeight="1">
-      <c r="A28" s="38"/>
+      <c r="A28" s="39"/>
       <c r="B28" s="25"/>
       <c r="C28" s="26" t="s">
         <v>23</v>
@@ -8183,11 +8183,11 @@
       <c r="F28" s="27"/>
       <c r="G28" s="7">
         <f>COUNTIF(D29:D36,"Sim")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H28" s="7">
         <f>COUNTIF(D29:D36,"Parcialmente")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28" s="7">
         <f>COUNTIF(D29:D36,"Não")</f>
@@ -8207,7 +8207,7 @@
         <v>45</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E29" s="30"/>
       <c r="F29" s="30"/>
@@ -8218,10 +8218,10 @@
         <v>22.0</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E30" s="30"/>
       <c r="F30" s="30"/>
@@ -8232,10 +8232,10 @@
         <v>23.0</v>
       </c>
       <c r="C31" s="30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E31" s="30"/>
       <c r="F31" s="30"/>
@@ -8246,10 +8246,10 @@
         <v>24.0</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E32" s="30"/>
       <c r="F32" s="30"/>
@@ -8260,10 +8260,10 @@
         <v>25.0</v>
       </c>
       <c r="C33" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E33" s="30"/>
       <c r="F33" s="30"/>
@@ -8274,10 +8274,10 @@
         <v>26.0</v>
       </c>
       <c r="C34" s="30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F34" s="30"/>
     </row>
@@ -8287,31 +8287,31 @@
         <v>27.0</v>
       </c>
       <c r="C35" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D35" s="31" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E35" s="30"/>
       <c r="F35" s="30"/>
     </row>
     <row r="36" ht="18.75" customHeight="1">
-      <c r="A36" s="37"/>
+      <c r="A36" s="38"/>
       <c r="B36" s="29">
         <v>28.0</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="D36" s="39" t="s">
-        <v>43</v>
+        <v>66</v>
+      </c>
+      <c r="D36" s="37" t="s">
+        <v>46</v>
       </c>
       <c r="E36" s="30"/>
       <c r="F36" s="30"/>
     </row>
     <row r="37" ht="15.0" customHeight="1">
       <c r="A37" s="40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B37" s="25"/>
       <c r="C37" s="26" t="s">
@@ -8326,7 +8326,7 @@
       </c>
       <c r="H37" s="7">
         <f>COUNTIF(D38:D41,"Parcialmente")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37" s="7">
         <f>COUNTIF(D38:D41,"Não")</f>
@@ -8334,7 +8334,7 @@
       </c>
       <c r="J37" s="7">
         <f>COUNTIF(D38:D41,"NA")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" ht="18.75" customHeight="1">
@@ -8343,10 +8343,10 @@
         <v>30.0</v>
       </c>
       <c r="C38" s="34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D38" s="31" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E38" s="30"/>
       <c r="F38" s="30"/>
@@ -8357,10 +8357,10 @@
         <v>31.0</v>
       </c>
       <c r="C39" s="30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D39" s="31" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E39" s="30"/>
       <c r="F39" s="30"/>
@@ -8371,10 +8371,10 @@
         <v>32.0</v>
       </c>
       <c r="C40" s="30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E40" s="30"/>
       <c r="F40" s="30"/>
@@ -8385,13 +8385,13 @@
         <v>33.0</v>
       </c>
       <c r="C41" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D41" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="D41" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="E41" s="30"/>
-      <c r="F41" s="30"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="37"/>
     </row>
     <row r="42" ht="18.75" customHeight="1">
       <c r="B42" s="43"/>
@@ -12352,7 +12352,7 @@
         <v>73</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
@@ -12459,7 +12459,7 @@
       <c r="A10" s="32"/>
       <c r="B10" s="25"/>
       <c r="C10" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10" s="27"/>
       <c r="E10" s="27"/>
@@ -12540,7 +12540,7 @@
       <c r="F15" s="27"/>
     </row>
     <row r="16" ht="18.75" customHeight="1">
-      <c r="A16" s="37"/>
+      <c r="A16" s="38"/>
       <c r="B16" s="29">
         <v>7.0</v>
       </c>
@@ -12652,7 +12652,7 @@
       <c r="Z20" s="35"/>
     </row>
     <row r="21" ht="18.75" customHeight="1">
-      <c r="A21" s="37"/>
+      <c r="A21" s="38"/>
       <c r="B21" s="29">
         <v>12.0</v>
       </c>
@@ -12740,7 +12740,7 @@
       <c r="F26" s="30"/>
     </row>
     <row r="27" ht="18.75" customHeight="1">
-      <c r="A27" s="37"/>
+      <c r="A27" s="38"/>
       <c r="B27" s="29">
         <v>22.0</v>
       </c>
@@ -12853,7 +12853,7 @@
     </row>
     <row r="35" ht="15.0" customHeight="1">
       <c r="A35" s="40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B35" s="25"/>
       <c r="C35" s="26" t="s">
@@ -12869,7 +12869,7 @@
         <v>29.0</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D36" s="48"/>
       <c r="E36" s="30"/>
@@ -12897,7 +12897,7 @@
         <v>30.0</v>
       </c>
       <c r="C37" s="30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D37" s="48"/>
       <c r="E37" s="30"/>
@@ -12909,7 +12909,7 @@
         <v>31.0</v>
       </c>
       <c r="C38" s="30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D38" s="48"/>
       <c r="E38" s="30"/>
@@ -17005,7 +17005,7 @@
       <c r="A9" s="32"/>
       <c r="B9" s="25"/>
       <c r="C9" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D9" s="27"/>
       <c r="E9" s="27"/>
@@ -17074,7 +17074,7 @@
       <c r="F13" s="27"/>
     </row>
     <row r="14" ht="18.75" customHeight="1">
-      <c r="A14" s="37"/>
+      <c r="A14" s="38"/>
       <c r="B14" s="29">
         <v>6.0</v>
       </c>
@@ -17114,7 +17114,7 @@
       <c r="F15" s="27"/>
     </row>
     <row r="16" ht="18.75" customHeight="1">
-      <c r="A16" s="37"/>
+      <c r="A16" s="38"/>
       <c r="B16" s="29">
         <v>8.0</v>
       </c>
@@ -17218,7 +17218,7 @@
       <c r="F21" s="30"/>
     </row>
     <row r="22" ht="18.75" customHeight="1">
-      <c r="A22" s="37"/>
+      <c r="A22" s="38"/>
       <c r="B22" s="29">
         <v>16.0</v>
       </c>
@@ -17306,7 +17306,7 @@
       <c r="F27" s="30"/>
     </row>
     <row r="28" ht="18.75" customHeight="1">
-      <c r="A28" s="37"/>
+      <c r="A28" s="38"/>
       <c r="B28" s="29">
         <v>22.0</v>
       </c>
@@ -17407,7 +17407,7 @@
     </row>
     <row r="35" ht="15.0" customHeight="1">
       <c r="A35" s="40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B35" s="25"/>
       <c r="C35" s="26" t="s">
@@ -17423,7 +17423,7 @@
         <v>30.0</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D36" s="48"/>
       <c r="E36" s="30"/>
@@ -17451,7 +17451,7 @@
         <v>31.0</v>
       </c>
       <c r="C37" s="30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D37" s="48"/>
       <c r="E37" s="30"/>
@@ -17463,7 +17463,7 @@
         <v>32.0</v>
       </c>
       <c r="C38" s="30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D38" s="48"/>
       <c r="E38" s="30"/>
@@ -21614,7 +21614,7 @@
       <c r="F13" s="27"/>
     </row>
     <row r="14" ht="18.75" customHeight="1">
-      <c r="A14" s="37"/>
+      <c r="A14" s="38"/>
       <c r="B14" s="29">
         <v>6.0</v>
       </c>
@@ -21654,7 +21654,7 @@
       <c r="F15" s="27"/>
     </row>
     <row r="16" ht="18.75" customHeight="1">
-      <c r="A16" s="37"/>
+      <c r="A16" s="38"/>
       <c r="B16" s="29">
         <v>8.0</v>
       </c>
@@ -21798,7 +21798,7 @@
       </c>
     </row>
     <row r="24" ht="18.75" customHeight="1">
-      <c r="A24" s="37"/>
+      <c r="A24" s="38"/>
       <c r="B24" s="29">
         <v>15.0</v>
       </c>
@@ -21928,7 +21928,7 @@
       <c r="F28" s="27"/>
     </row>
     <row r="29" ht="18.75" customHeight="1">
-      <c r="A29" s="37"/>
+      <c r="A29" s="38"/>
       <c r="B29" s="36">
         <v>26.0</v>
       </c>
@@ -22045,7 +22045,7 @@
     </row>
     <row r="36" ht="15.0" customHeight="1">
       <c r="A36" s="40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B36" s="25"/>
       <c r="C36" s="26" t="s">
@@ -22061,7 +22061,7 @@
         <v>26.0</v>
       </c>
       <c r="C37" s="30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D37" s="48"/>
       <c r="E37" s="30"/>
@@ -22089,7 +22089,7 @@
         <v>27.0</v>
       </c>
       <c r="C38" s="30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D38" s="48"/>
       <c r="E38" s="30"/>
@@ -22101,7 +22101,7 @@
         <v>28.0</v>
       </c>
       <c r="C39" s="30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D39" s="48"/>
       <c r="E39" s="30"/>

</xml_diff>